<commit_message>
Revert "removed main etc."
This reverts commit c5289b1b09859a263af0c420cafd20ab36661507.
</commit_message>
<xml_diff>
--- a/results/test_excel/test_excel.xlsx
+++ b/results/test_excel/test_excel.xlsx
@@ -467,7 +467,7 @@
     <t>30.09.2011</t>
   </si>
   <si>
-    <t>05.10.2011</t>
+    <t>15.10.2011</t>
   </si>
 </sst>
 </file>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A226" sqref="A226"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1600,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C83">
         <v>1</v>

</xml_diff>